<commit_message>
CREATE: Change name partner and add percent partner
</commit_message>
<xml_diff>
--- a/Planilhas/AlteracaoNomeParceiros.xlsx
+++ b/Planilhas/AlteracaoNomeParceiros.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonatan.azevedo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tributo\FilterContract\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C6A0ED-E867-40D6-823F-28ED34B41C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0748E1-26F9-4FFE-B0CB-C15E0AB12151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E5FBF92-2A4F-42A1-9937-E5C7BB6B6073}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4E5FBF92-2A4F-42A1-9937-E5C7BB6B6073}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
   <si>
     <t>Nome novo</t>
   </si>
@@ -292,15 +292,103 @@
   </si>
   <si>
     <t>NASCIMENTO NAVARRO CONTABILIDADE &amp; CONSULTORIA LTDA</t>
+  </si>
+  <si>
+    <t>SR. RENATO/ BRANCA DE JESUS</t>
+  </si>
+  <si>
+    <t>EMANUEL/ ROSETTI CORP</t>
+  </si>
+  <si>
+    <t>IVO/ AUTO POSTO TRANSYARA</t>
+  </si>
+  <si>
+    <t>MARINA/ EMANUEL</t>
+  </si>
+  <si>
+    <t>JOSÉ / JULIA COLLE</t>
+  </si>
+  <si>
+    <t>ORLANDO/ DANIELA</t>
+  </si>
+  <si>
+    <t>SINDIPETRO/ EMANUEL</t>
+  </si>
+  <si>
+    <t>THYAGO/ EMANUEL</t>
+  </si>
+  <si>
+    <t>SINDIPETRO PB / EMANUEL</t>
+  </si>
+  <si>
+    <t>MAC CONSULT MANAUS/ WALTER</t>
+  </si>
+  <si>
+    <t>JAIRO/KLEYTON</t>
+  </si>
+  <si>
+    <t>MARCELE POIANI / BESS</t>
+  </si>
+  <si>
+    <t>THARYK / BESS DAGOBERTO</t>
+  </si>
+  <si>
+    <t>BESS / DAGOBERTO</t>
+  </si>
+  <si>
+    <t>TIME JUNIOR LEITE/ FIORI-ANNONI</t>
+  </si>
+  <si>
+    <t>IGNACIO/EMANUEL</t>
+  </si>
+  <si>
+    <t>SINPETRO MS / EMANUEL</t>
+  </si>
+  <si>
+    <t>GLAVO/ FSC</t>
+  </si>
+  <si>
+    <t>JORGE DOMINGOS/ANNONI</t>
+  </si>
+  <si>
+    <t>ASSOHONDA / ANNONI</t>
+  </si>
+  <si>
+    <t>JAIRO EQUIPE LONDRINA/KLEYTON</t>
+  </si>
+  <si>
+    <t>DSM3 PROJETOS  / ANNONI</t>
+  </si>
+  <si>
+    <t>SABRINA MARCOLLI / BESS</t>
+  </si>
+  <si>
+    <t>NN CONTABILIDADE / BESS</t>
+  </si>
+  <si>
+    <t>SR. RENATO- BRANCA DE JESUS</t>
+  </si>
+  <si>
+    <t>EDUARDO/ DANIELA EURO VICIELI</t>
+  </si>
+  <si>
+    <t>LAURO MONTEIRO NETO/ Afonso (ANNONI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -321,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -329,14 +417,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,19 +766,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69A1100-7CF9-47A4-87C0-D8EF3934074B}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -671,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -679,353 +794,569 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B43" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B45" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B49" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B55" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>69</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>71</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>73</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>78</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B65" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>80</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>82</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B68" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B70" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>86</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B72" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B44" xr:uid="{F69A1100-7CF9-47A4-87C0-D8EF3934074B}"/>
+  <autoFilter ref="A1:B70" xr:uid="{F69A1100-7CF9-47A4-87C0-D8EF3934074B}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>